<commit_message>
2020/10/29 edit by he.chao
</commit_message>
<xml_diff>
--- a/testcase/middleground/caseData/caseData_sectionAdd.xlsx
+++ b/testcase/middleground/caseData/caseData_sectionAdd.xlsx
@@ -4,17 +4,18 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="25417" windowHeight="11112"/>
+    <workbookView windowWidth="25417" windowHeight="11112" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="sectionAdd" sheetId="1" r:id="rId1"/>
+    <sheet name="sectionPageList" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="144525"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="182" uniqueCount="84">
   <si>
     <t>case_no</t>
   </si>
@@ -22,10 +23,10 @@
     <t>case_title</t>
   </si>
   <si>
-    <t>业务模块</t>
-  </si>
-  <si>
-    <t>接口</t>
+    <t>modular</t>
+  </si>
+  <si>
+    <t>interface</t>
   </si>
   <si>
     <t>case_data</t>
@@ -34,7 +35,7 @@
     <t>case_expect</t>
   </si>
   <si>
-    <t>正常创建</t>
+    <t>正常创建号段</t>
   </si>
   <si>
     <t xml:space="preserve">号段管理 </t>
@@ -44,9 +45,6 @@
   </si>
   <si>
     <t>{'prefix':'#prefix#','bizId':1,'num':#num#}</t>
-  </si>
-  <si>
-    <t>{"prefix":'#prefix#',"bizId":1,"num":#num#}</t>
   </si>
   <si>
     <t>前缀prefix为特殊字符</t>
@@ -182,6 +180,111 @@
   </si>
   <si>
     <t>{'prefix':'#prefix#','bizId':1,'num':'!'}</t>
+  </si>
+  <si>
+    <t>正常查询号段</t>
+  </si>
+  <si>
+    <t>{"pn":1,"ps":5}</t>
+  </si>
+  <si>
+    <t>页数pn为0</t>
+  </si>
+  <si>
+    <t>{"pn":0,"ps":#ps#}</t>
+  </si>
+  <si>
+    <t>{"pn":1,"ps":#ps#}</t>
+  </si>
+  <si>
+    <t>页数pn为空</t>
+  </si>
+  <si>
+    <t>{"pn":"","ps":#ps#}</t>
+  </si>
+  <si>
+    <t>页数pn为空格</t>
+  </si>
+  <si>
+    <t>{"pn":" ","ps":#ps#}</t>
+  </si>
+  <si>
+    <t>页数pn为小数</t>
+  </si>
+  <si>
+    <t>{"pn":1.1,"ps":#ps#}</t>
+  </si>
+  <si>
+    <t>页数pn为字符</t>
+  </si>
+  <si>
+    <t>{"pn":"a","ps":#ps#}</t>
+  </si>
+  <si>
+    <t>页数pn为特殊字符</t>
+  </si>
+  <si>
+    <t>{"pn":"!","ps":#ps#}</t>
+  </si>
+  <si>
+    <t>页数pn为负数</t>
+  </si>
+  <si>
+    <t>{"pn":-1,"ps":#ps#}</t>
+  </si>
+  <si>
+    <t>页数pn为极大值</t>
+  </si>
+  <si>
+    <t>{"pn":100000000000000000,"ps":#ps#}</t>
+  </si>
+  <si>
+    <t>每页显示数量ps为0</t>
+  </si>
+  <si>
+    <t>{"pn":#pn#,"ps":0}</t>
+  </si>
+  <si>
+    <t>{"pn":#pn#,"ps":20}</t>
+  </si>
+  <si>
+    <t>每页显示数量ps为空</t>
+  </si>
+  <si>
+    <t>{"pn":#pn#,"ps":""}</t>
+  </si>
+  <si>
+    <t>每页显示数量ps为空格</t>
+  </si>
+  <si>
+    <t>每页显示数量ps为小数</t>
+  </si>
+  <si>
+    <t>{"pn":#pn#,"ps":5.1}</t>
+  </si>
+  <si>
+    <t>每页显示数量ps为字符</t>
+  </si>
+  <si>
+    <t>{"pn":#pn#,"ps":"a"}</t>
+  </si>
+  <si>
+    <t>每页显示数量ps为特殊字符</t>
+  </si>
+  <si>
+    <t>{"pn":#pn#,"ps":"!"}</t>
+  </si>
+  <si>
+    <t>每页显示数量ps为负数</t>
+  </si>
+  <si>
+    <t>{"pn":#pn#,"ps":-1}</t>
+  </si>
+  <si>
+    <t>每页显示数量ps为极大值</t>
+  </si>
+  <si>
+    <t>{"pn":#pn#,"ps":10000000000000}</t>
   </si>
 </sst>
 </file>
@@ -189,10 +292,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
+    <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
   </numFmts>
   <fonts count="20">
     <font>
@@ -204,28 +307,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color theme="0"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
       <color rgb="FFFA7D00"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -238,32 +320,15 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
       <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
+      <color rgb="FFFF0000"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <b/>
-      <sz val="15"/>
+      <sz val="11"/>
       <color theme="3"/>
       <name val="宋体"/>
       <charset val="134"/>
@@ -278,18 +343,17 @@
     </font>
     <font>
       <b/>
-      <sz val="18"/>
+      <sz val="13"/>
       <color theme="3"/>
       <name val="宋体"/>
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
       <sz val="11"/>
-      <color theme="3"/>
+      <color theme="1"/>
       <name val="宋体"/>
-      <charset val="134"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -300,11 +364,49 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
-      <sz val="13"/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
       <color theme="3"/>
       <name val="宋体"/>
       <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="宋体"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -325,6 +427,14 @@
     </font>
     <font>
       <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="11"/>
       <color rgb="FFFFFFFF"/>
       <name val="宋体"/>
@@ -332,16 +442,9 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
+      <color rgb="FFFA7D00"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -356,54 +459,180 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="8"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="6"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="4" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="4" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
@@ -411,132 +640,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -555,6 +658,21 @@
       <top/>
       <bottom style="double">
         <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
       </bottom>
       <diagonal/>
     </border>
@@ -584,16 +702,16 @@
     </border>
     <border>
       <left style="thin">
-        <color rgb="FFB2B2B2"/>
+        <color rgb="FF3F3F3F"/>
       </left>
       <right style="thin">
-        <color rgb="FFB2B2B2"/>
+        <color rgb="FF3F3F3F"/>
       </right>
       <top style="thin">
-        <color rgb="FFB2B2B2"/>
+        <color rgb="FF3F3F3F"/>
       </top>
       <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
+        <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -605,6 +723,15 @@
       </top>
       <bottom style="double">
         <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
       </bottom>
       <diagonal/>
     </border>
@@ -623,30 +750,6 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
@@ -655,10 +758,10 @@
     <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="14" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -667,133 +770,133 @@
     <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="21" borderId="4" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="8" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="8" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="24" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="17" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="17" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="29" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -1125,14 +1228,15 @@
   <sheetPr/>
   <dimension ref="A1:F18"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E9" sqref="E9"/>
+    <sheetView topLeftCell="A11" workbookViewId="0">
+      <selection activeCell="C21" sqref="C21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.99082568807339" defaultRowHeight="12.9" outlineLevelCol="5"/>
   <cols>
     <col min="2" max="2" width="26.1651376146789" customWidth="1"/>
-    <col min="3" max="4" width="19.4128440366972" customWidth="1"/>
+    <col min="3" max="3" width="19.4128440366972" customWidth="1"/>
+    <col min="4" max="4" width="20.6146788990826" customWidth="1"/>
     <col min="5" max="5" width="71.5412844036697" customWidth="1"/>
     <col min="6" max="6" width="69.0366972477064" customWidth="1"/>
   </cols>
@@ -1174,7 +1278,7 @@
         <v>9</v>
       </c>
       <c r="F2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="3" spans="1:6">
@@ -1182,19 +1286,19 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
+        <v>10</v>
+      </c>
+      <c r="C3" t="s">
+        <v>7</v>
+      </c>
+      <c r="D3" t="s">
+        <v>8</v>
+      </c>
+      <c r="E3" t="s">
         <v>11</v>
       </c>
-      <c r="C3" t="s">
-        <v>7</v>
-      </c>
-      <c r="D3" t="s">
-        <v>8</v>
-      </c>
-      <c r="E3" t="s">
-        <v>12</v>
-      </c>
       <c r="F3" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="4" spans="1:6">
@@ -1202,19 +1306,19 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
+        <v>12</v>
+      </c>
+      <c r="C4" t="s">
+        <v>7</v>
+      </c>
+      <c r="D4" t="s">
+        <v>8</v>
+      </c>
+      <c r="E4" t="s">
         <v>13</v>
       </c>
-      <c r="C4" t="s">
-        <v>7</v>
-      </c>
-      <c r="D4" t="s">
-        <v>8</v>
-      </c>
-      <c r="E4" t="s">
-        <v>14</v>
-      </c>
       <c r="F4" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="5" spans="1:6">
@@ -1222,19 +1326,19 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
+        <v>14</v>
+      </c>
+      <c r="C5" t="s">
+        <v>7</v>
+      </c>
+      <c r="D5" t="s">
+        <v>8</v>
+      </c>
+      <c r="E5" t="s">
         <v>15</v>
       </c>
-      <c r="C5" t="s">
-        <v>7</v>
-      </c>
-      <c r="D5" t="s">
-        <v>8</v>
-      </c>
-      <c r="E5" t="s">
+      <c r="F5" t="s">
         <v>16</v>
-      </c>
-      <c r="F5" t="s">
-        <v>17</v>
       </c>
     </row>
     <row r="6" ht="25.8" spans="1:6">
@@ -1242,19 +1346,19 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
+        <v>17</v>
+      </c>
+      <c r="C6" t="s">
+        <v>7</v>
+      </c>
+      <c r="D6" t="s">
+        <v>8</v>
+      </c>
+      <c r="E6" t="s">
         <v>18</v>
       </c>
-      <c r="C6" t="s">
-        <v>7</v>
-      </c>
-      <c r="D6" t="s">
-        <v>8</v>
-      </c>
-      <c r="E6" t="s">
-        <v>19</v>
-      </c>
       <c r="F6" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="7" spans="1:6">
@@ -1262,19 +1366,19 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
+        <v>19</v>
+      </c>
+      <c r="C7" t="s">
+        <v>7</v>
+      </c>
+      <c r="D7" t="s">
+        <v>8</v>
+      </c>
+      <c r="E7" t="s">
         <v>20</v>
       </c>
-      <c r="C7" t="s">
-        <v>7</v>
-      </c>
-      <c r="D7" t="s">
-        <v>8</v>
-      </c>
-      <c r="E7" t="s">
+      <c r="F7" t="s">
         <v>21</v>
-      </c>
-      <c r="F7" t="s">
-        <v>22</v>
       </c>
     </row>
     <row r="8" spans="1:6">
@@ -1282,208 +1386,593 @@
         <v>7</v>
       </c>
       <c r="B8" t="s">
+        <v>22</v>
+      </c>
+      <c r="C8" t="s">
+        <v>7</v>
+      </c>
+      <c r="D8" t="s">
+        <v>8</v>
+      </c>
+      <c r="E8" t="s">
         <v>23</v>
       </c>
-      <c r="C8" t="s">
-        <v>7</v>
-      </c>
-      <c r="D8" t="s">
-        <v>8</v>
-      </c>
-      <c r="E8" t="s">
-        <v>24</v>
-      </c>
       <c r="F8" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="9" ht="64.55" spans="1:6">
       <c r="A9">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B9" t="s">
+        <v>24</v>
+      </c>
+      <c r="C9" t="s">
+        <v>7</v>
+      </c>
+      <c r="D9" t="s">
+        <v>8</v>
+      </c>
+      <c r="E9" t="s">
         <v>25</v>
       </c>
-      <c r="C9" t="s">
-        <v>7</v>
-      </c>
-      <c r="D9" t="s">
-        <v>8</v>
-      </c>
-      <c r="E9" t="s">
+      <c r="F9" s="1" t="s">
         <v>26</v>
-      </c>
-      <c r="F9" s="1" t="s">
-        <v>27</v>
       </c>
     </row>
     <row r="10" ht="64.55" spans="1:6">
       <c r="A10">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B10" t="s">
+        <v>27</v>
+      </c>
+      <c r="C10" t="s">
+        <v>7</v>
+      </c>
+      <c r="D10" t="s">
+        <v>8</v>
+      </c>
+      <c r="E10" t="s">
         <v>28</v>
       </c>
-      <c r="C10" t="s">
-        <v>7</v>
-      </c>
-      <c r="D10" t="s">
-        <v>8</v>
-      </c>
-      <c r="E10" t="s">
-        <v>29</v>
-      </c>
       <c r="F10" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="11" ht="64.55" spans="1:6">
       <c r="A11">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B11" t="s">
+        <v>29</v>
+      </c>
+      <c r="C11" t="s">
+        <v>7</v>
+      </c>
+      <c r="D11" t="s">
+        <v>8</v>
+      </c>
+      <c r="E11" t="s">
         <v>30</v>
       </c>
-      <c r="C11" t="s">
-        <v>7</v>
-      </c>
-      <c r="D11" t="s">
-        <v>8</v>
-      </c>
-      <c r="E11" t="s">
+      <c r="F11" s="1" t="s">
         <v>31</v>
-      </c>
-      <c r="F11" s="1" t="s">
-        <v>32</v>
       </c>
     </row>
     <row r="12" ht="64.55" spans="1:6">
       <c r="A12">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B12" t="s">
+        <v>32</v>
+      </c>
+      <c r="C12" t="s">
+        <v>7</v>
+      </c>
+      <c r="D12" t="s">
+        <v>8</v>
+      </c>
+      <c r="E12" t="s">
         <v>33</v>
       </c>
-      <c r="C12" t="s">
-        <v>7</v>
-      </c>
-      <c r="D12" t="s">
-        <v>8</v>
-      </c>
-      <c r="E12" t="s">
-        <v>34</v>
-      </c>
       <c r="F12" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="13" ht="38.7" spans="1:6">
       <c r="A13">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B13" t="s">
+        <v>34</v>
+      </c>
+      <c r="C13" t="s">
+        <v>7</v>
+      </c>
+      <c r="D13" t="s">
+        <v>8</v>
+      </c>
+      <c r="E13" t="s">
         <v>35</v>
       </c>
-      <c r="C13" t="s">
-        <v>7</v>
-      </c>
-      <c r="D13" t="s">
-        <v>8</v>
-      </c>
-      <c r="E13" t="s">
+      <c r="F13" s="1" t="s">
         <v>36</v>
-      </c>
-      <c r="F13" s="1" t="s">
-        <v>37</v>
       </c>
     </row>
     <row r="14" ht="64.55" spans="1:6">
       <c r="A14">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B14" t="s">
+        <v>37</v>
+      </c>
+      <c r="C14" t="s">
+        <v>7</v>
+      </c>
+      <c r="D14" t="s">
+        <v>8</v>
+      </c>
+      <c r="E14" t="s">
         <v>38</v>
       </c>
-      <c r="C14" t="s">
-        <v>7</v>
-      </c>
-      <c r="D14" t="s">
-        <v>8</v>
-      </c>
-      <c r="E14" t="s">
+      <c r="F14" s="1" t="s">
         <v>39</v>
-      </c>
-      <c r="F14" s="1" t="s">
-        <v>40</v>
       </c>
     </row>
     <row r="15" ht="64.55" spans="1:6">
       <c r="A15">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B15" t="s">
+        <v>40</v>
+      </c>
+      <c r="C15" t="s">
+        <v>7</v>
+      </c>
+      <c r="D15" t="s">
+        <v>8</v>
+      </c>
+      <c r="E15" t="s">
         <v>41</v>
       </c>
-      <c r="C15" t="s">
-        <v>7</v>
-      </c>
-      <c r="D15" t="s">
-        <v>8</v>
-      </c>
-      <c r="E15" t="s">
+      <c r="F15" s="1" t="s">
         <v>42</v>
-      </c>
-      <c r="F15" s="1" t="s">
-        <v>43</v>
       </c>
     </row>
     <row r="16" ht="64.55" spans="1:6">
       <c r="A16">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B16" t="s">
+        <v>43</v>
+      </c>
+      <c r="C16" t="s">
+        <v>7</v>
+      </c>
+      <c r="D16" t="s">
+        <v>8</v>
+      </c>
+      <c r="E16" t="s">
         <v>44</v>
       </c>
-      <c r="C16" t="s">
-        <v>7</v>
-      </c>
-      <c r="D16" t="s">
-        <v>8</v>
-      </c>
-      <c r="E16" t="s">
-        <v>45</v>
-      </c>
       <c r="F16" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="17" ht="38.7" spans="1:6">
       <c r="A17">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B17" t="s">
+        <v>45</v>
+      </c>
+      <c r="C17" t="s">
+        <v>7</v>
+      </c>
+      <c r="D17" t="s">
+        <v>8</v>
+      </c>
+      <c r="E17" t="s">
         <v>46</v>
       </c>
-      <c r="C17" t="s">
-        <v>7</v>
-      </c>
-      <c r="D17" t="s">
-        <v>8</v>
-      </c>
-      <c r="E17" t="s">
-        <v>47</v>
-      </c>
       <c r="F17" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="18" ht="38.7" spans="1:6">
       <c r="A18">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B18" t="s">
+        <v>47</v>
+      </c>
+      <c r="C18" t="s">
+        <v>7</v>
+      </c>
+      <c r="D18" t="s">
+        <v>8</v>
+      </c>
+      <c r="E18" t="s">
         <v>48</v>
       </c>
+      <c r="F18" s="1" t="s">
+        <v>36</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <headerFooter/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
+  <dimension ref="A1:F18"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E11" sqref="E11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="8.99082568807339" defaultRowHeight="12.9" outlineLevelCol="5"/>
+  <cols>
+    <col min="1" max="1" width="8.4954128440367" customWidth="1"/>
+    <col min="2" max="2" width="27.256880733945" customWidth="1"/>
+    <col min="3" max="3" width="9.45871559633028" customWidth="1"/>
+    <col min="4" max="4" width="20.6146788990826" customWidth="1"/>
+    <col min="5" max="5" width="39.7339449541284" customWidth="1"/>
+    <col min="6" max="6" width="46.605504587156" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
+        <v>49</v>
+      </c>
+      <c r="C2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E2" t="s">
+        <v>50</v>
+      </c>
+      <c r="F2" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3" t="s">
+        <v>51</v>
+      </c>
+      <c r="C3" t="s">
+        <v>7</v>
+      </c>
+      <c r="D3" t="s">
+        <v>8</v>
+      </c>
+      <c r="E3" t="s">
+        <v>52</v>
+      </c>
+      <c r="F3" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4" t="s">
+        <v>54</v>
+      </c>
+      <c r="C4" t="s">
+        <v>7</v>
+      </c>
+      <c r="D4" t="s">
+        <v>8</v>
+      </c>
+      <c r="E4" t="s">
+        <v>55</v>
+      </c>
+      <c r="F4" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5" t="s">
+        <v>56</v>
+      </c>
+      <c r="C5" t="s">
+        <v>7</v>
+      </c>
+      <c r="D5" t="s">
+        <v>8</v>
+      </c>
+      <c r="E5" t="s">
+        <v>57</v>
+      </c>
+      <c r="F5" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="6" ht="38.7" spans="1:6">
+      <c r="A6">
+        <v>5</v>
+      </c>
+      <c r="B6" t="s">
+        <v>58</v>
+      </c>
+      <c r="C6" t="s">
+        <v>7</v>
+      </c>
+      <c r="D6" t="s">
+        <v>8</v>
+      </c>
+      <c r="E6" t="s">
+        <v>59</v>
+      </c>
+      <c r="F6" s="1" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="7" ht="38.7" spans="1:6">
+      <c r="A7">
+        <v>6</v>
+      </c>
+      <c r="B7" t="s">
+        <v>60</v>
+      </c>
+      <c r="C7" t="s">
+        <v>7</v>
+      </c>
+      <c r="D7" t="s">
+        <v>8</v>
+      </c>
+      <c r="E7" t="s">
+        <v>61</v>
+      </c>
+      <c r="F7" s="1" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="8" ht="38.7" spans="1:6">
+      <c r="A8">
+        <v>7</v>
+      </c>
+      <c r="B8" t="s">
+        <v>62</v>
+      </c>
+      <c r="C8" t="s">
+        <v>7</v>
+      </c>
+      <c r="D8" t="s">
+        <v>8</v>
+      </c>
+      <c r="E8" t="s">
+        <v>63</v>
+      </c>
+      <c r="F8" s="1" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="9" ht="38.7" spans="1:6">
+      <c r="A9">
+        <v>8</v>
+      </c>
+      <c r="B9" t="s">
+        <v>64</v>
+      </c>
+      <c r="C9" t="s">
+        <v>7</v>
+      </c>
+      <c r="D9" t="s">
+        <v>8</v>
+      </c>
+      <c r="E9" t="s">
+        <v>65</v>
+      </c>
+      <c r="F9" s="1" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="10" ht="38.7" spans="1:6">
+      <c r="A10">
+        <v>9</v>
+      </c>
+      <c r="B10" t="s">
+        <v>66</v>
+      </c>
+      <c r="C10" t="s">
+        <v>7</v>
+      </c>
+      <c r="D10" t="s">
+        <v>8</v>
+      </c>
+      <c r="E10" t="s">
+        <v>67</v>
+      </c>
+      <c r="F10" s="1" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6">
+      <c r="A11">
+        <v>10</v>
+      </c>
+      <c r="B11" t="s">
+        <v>68</v>
+      </c>
+      <c r="C11" t="s">
+        <v>7</v>
+      </c>
+      <c r="D11" t="s">
+        <v>8</v>
+      </c>
+      <c r="E11" t="s">
+        <v>69</v>
+      </c>
+      <c r="F11" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6">
+      <c r="A12">
+        <v>11</v>
+      </c>
+      <c r="B12" t="s">
+        <v>71</v>
+      </c>
+      <c r="C12" t="s">
+        <v>7</v>
+      </c>
+      <c r="D12" t="s">
+        <v>8</v>
+      </c>
+      <c r="E12" t="s">
+        <v>72</v>
+      </c>
+      <c r="F12" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6">
+      <c r="A13">
+        <v>12</v>
+      </c>
+      <c r="B13" t="s">
+        <v>73</v>
+      </c>
+      <c r="C13" t="s">
+        <v>7</v>
+      </c>
+      <c r="D13" t="s">
+        <v>8</v>
+      </c>
+      <c r="E13" t="s">
+        <v>72</v>
+      </c>
+      <c r="F13" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="14" ht="38.7" spans="1:6">
+      <c r="A14">
+        <v>13</v>
+      </c>
+      <c r="B14" t="s">
+        <v>74</v>
+      </c>
+      <c r="C14" t="s">
+        <v>7</v>
+      </c>
+      <c r="D14" t="s">
+        <v>8</v>
+      </c>
+      <c r="E14" t="s">
+        <v>75</v>
+      </c>
+      <c r="F14" s="1" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="15" ht="38.7" spans="1:6">
+      <c r="A15">
+        <v>14</v>
+      </c>
+      <c r="B15" t="s">
+        <v>76</v>
+      </c>
+      <c r="C15" t="s">
+        <v>7</v>
+      </c>
+      <c r="D15" t="s">
+        <v>8</v>
+      </c>
+      <c r="E15" t="s">
+        <v>77</v>
+      </c>
+      <c r="F15" s="1" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="16" ht="38.7" spans="1:6">
+      <c r="A16">
+        <v>15</v>
+      </c>
+      <c r="B16" t="s">
+        <v>78</v>
+      </c>
+      <c r="C16" t="s">
+        <v>7</v>
+      </c>
+      <c r="D16" t="s">
+        <v>8</v>
+      </c>
+      <c r="E16" t="s">
+        <v>79</v>
+      </c>
+      <c r="F16" s="1" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="17" ht="38.7" spans="1:6">
+      <c r="A17">
+        <v>16</v>
+      </c>
+      <c r="B17" t="s">
+        <v>80</v>
+      </c>
+      <c r="C17" t="s">
+        <v>7</v>
+      </c>
+      <c r="D17" t="s">
+        <v>8</v>
+      </c>
+      <c r="E17" t="s">
+        <v>81</v>
+      </c>
+      <c r="F17" s="1" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="18" ht="38.7" spans="1:6">
+      <c r="A18">
+        <v>17</v>
+      </c>
+      <c r="B18" t="s">
+        <v>82</v>
+      </c>
       <c r="C18" t="s">
         <v>7</v>
       </c>
@@ -1491,10 +1980,10 @@
         <v>8</v>
       </c>
       <c r="E18" t="s">
-        <v>49</v>
+        <v>83</v>
       </c>
       <c r="F18" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
brandMP.py cartAdd.py case_data.py caseData_sectionAdd.xlsx config.yaml goodsMP.py middleground.py releaseSku.py sku_inventoryMP.py
</commit_message>
<xml_diff>
--- a/testcase/middleground/caseData/caseData_sectionAdd.xlsx
+++ b/testcase/middleground/caseData/caseData_sectionAdd.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="25417" windowHeight="11112"/>
+    <workbookView windowWidth="23040" windowHeight="9420"/>
   </bookViews>
   <sheets>
     <sheet name="sectionAdd" sheetId="1" r:id="rId1"/>
@@ -189,8 +189,8 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
+    <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
   </numFmts>
@@ -211,12 +211,119 @@
     </font>
     <font>
       <sz val="11"/>
+      <color theme="1"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
       <color rgb="FFFA7D00"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="宋体"/>
@@ -224,39 +331,9 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
+      <color rgb="FF3F3F3F"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -269,83 +346,6 @@
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
   <fills count="33">
     <fill>
@@ -362,181 +362,181 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="6"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="8" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -547,15 +547,6 @@
       <right/>
       <top/>
       <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
-      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -578,33 +569,25 @@
       <right/>
       <top/>
       <bottom style="medium">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FFB2B2B2"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFB2B2B2"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
+        <color theme="4" tint="0.499984740745262"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left/>
       <right/>
-      <top style="thin">
+      <top/>
+      <bottom style="medium">
         <color theme="4"/>
-      </top>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
       <bottom style="double">
-        <color theme="4"/>
+        <color rgb="FFFF8001"/>
       </bottom>
       <diagonal/>
     </border>
@@ -626,9 +609,11 @@
     <border>
       <left/>
       <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -647,6 +632,21 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
@@ -655,10 +655,10 @@
     <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="14" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="2" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="9" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -667,37 +667,37 @@
     <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="21" borderId="4" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="32" borderId="8" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -706,94 +706,94 @@
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="8" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="8" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="24" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="1" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="4" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="24" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="2" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="2" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -1125,16 +1125,16 @@
   <sheetPr/>
   <dimension ref="A1:F18"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E9" sqref="E9"/>
+    <sheetView tabSelected="1" topLeftCell="B15" workbookViewId="0">
+      <selection activeCell="F18" sqref="F18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.99082568807339" defaultRowHeight="12.9" outlineLevelCol="5"/>
+  <sheetFormatPr defaultColWidth="8.99074074074074" defaultRowHeight="14.4" outlineLevelCol="5"/>
   <cols>
-    <col min="2" max="2" width="26.1651376146789" customWidth="1"/>
-    <col min="3" max="4" width="19.4128440366972" customWidth="1"/>
-    <col min="5" max="5" width="71.5412844036697" customWidth="1"/>
-    <col min="6" max="6" width="69.0366972477064" customWidth="1"/>
+    <col min="2" max="2" width="26.1666666666667" customWidth="1"/>
+    <col min="3" max="4" width="19.4166666666667" customWidth="1"/>
+    <col min="5" max="5" width="71.537037037037" customWidth="1"/>
+    <col min="6" max="6" width="69.037037037037" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6">
@@ -1237,7 +1237,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="6" ht="25.8" spans="1:6">
+    <row r="6" ht="28.8" spans="1:6">
       <c r="A6">
         <v>5</v>
       </c>
@@ -1297,7 +1297,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="9" ht="64.55" spans="1:6">
+    <row r="9" ht="72" spans="1:6">
       <c r="A9">
         <v>9</v>
       </c>
@@ -1317,7 +1317,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="10" ht="64.55" spans="1:6">
+    <row r="10" ht="72" spans="1:6">
       <c r="A10">
         <v>10</v>
       </c>
@@ -1337,7 +1337,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="11" ht="64.55" spans="1:6">
+    <row r="11" ht="72" spans="1:6">
       <c r="A11">
         <v>11</v>
       </c>
@@ -1357,7 +1357,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="12" ht="64.55" spans="1:6">
+    <row r="12" ht="72" spans="1:6">
       <c r="A12">
         <v>12</v>
       </c>
@@ -1377,7 +1377,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="13" ht="38.7" spans="1:6">
+    <row r="13" ht="43.2" spans="1:6">
       <c r="A13">
         <v>13</v>
       </c>
@@ -1397,7 +1397,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="14" ht="64.55" spans="1:6">
+    <row r="14" ht="72" spans="1:6">
       <c r="A14">
         <v>14</v>
       </c>
@@ -1417,7 +1417,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="15" ht="64.55" spans="1:6">
+    <row r="15" ht="72" spans="1:6">
       <c r="A15">
         <v>15</v>
       </c>
@@ -1437,7 +1437,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="16" ht="64.55" spans="1:6">
+    <row r="16" ht="72" spans="1:6">
       <c r="A16">
         <v>16</v>
       </c>
@@ -1457,7 +1457,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="17" ht="38.7" spans="1:6">
+    <row r="17" ht="43.2" spans="1:6">
       <c r="A17">
         <v>17</v>
       </c>
@@ -1477,7 +1477,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="18" ht="38.7" spans="1:6">
+    <row r="18" ht="43.2" spans="1:6">
       <c r="A18">
         <v>18</v>
       </c>

</xml_diff>

<commit_message>
brandManage.py case_api.py case_data.py caseData_sectionAdd.xlsx inventory.py middleground.py shopManage.py skuManage.py tagManage.py
</commit_message>
<xml_diff>
--- a/testcase/middleground/caseData/caseData_sectionAdd.xlsx
+++ b/testcase/middleground/caseData/caseData_sectionAdd.xlsx
@@ -190,8 +190,8 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
     <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
   </numFmts>
   <fonts count="20">
@@ -204,6 +204,13 @@
     </font>
     <font>
       <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color theme="0"/>
       <name val="宋体"/>
       <charset val="0"/>
@@ -217,8 +224,30 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
       <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
       <color rgb="FFFA7D00"/>
       <name val="宋体"/>
       <charset val="0"/>
@@ -233,6 +262,22 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
       <color rgb="FF3F3F76"/>
       <name val="宋体"/>
@@ -240,22 +285,9 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -270,6 +302,13 @@
     </font>
     <font>
       <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color rgb="FFFA7D00"/>
       <name val="宋体"/>
       <charset val="0"/>
@@ -277,63 +316,24 @@
     </font>
     <font>
       <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <charset val="134"/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="宋体"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <u/>
       <sz val="11"/>
-      <color rgb="FF0000FF"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
       <color rgb="FF800080"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -356,187 +356,187 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="8"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -547,6 +547,21 @@
       <right/>
       <top/>
       <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -570,6 +585,17 @@
       <top/>
       <bottom style="medium">
         <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -607,32 +633,6 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left style="thin">
         <color rgb="FFB2B2B2"/>
       </left>
@@ -655,145 +655,145 @@
     <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="11" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="9" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="32" borderId="8" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="26" borderId="8" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="4" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="24" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="8" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="8" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="19" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -1125,8 +1125,8 @@
   <sheetPr/>
   <dimension ref="A1:F18"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B15" workbookViewId="0">
-      <selection activeCell="F18" sqref="F18"/>
+    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="E26" sqref="E26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.99074074074074" defaultRowHeight="14.4" outlineLevelCol="5"/>
@@ -1157,7 +1157,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:6">
+    <row r="2" ht="30" customHeight="1" spans="1:6">
       <c r="A2">
         <v>1</v>
       </c>
@@ -1177,7 +1177,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="3" spans="1:6">
+    <row r="3" ht="30" customHeight="1" spans="1:6">
       <c r="A3">
         <v>2</v>
       </c>
@@ -1197,7 +1197,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="4" spans="1:6">
+    <row r="4" ht="30" customHeight="1" spans="1:6">
       <c r="A4">
         <v>3</v>
       </c>
@@ -1217,7 +1217,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="5" spans="1:6">
+    <row r="5" ht="30" customHeight="1" spans="1:6">
       <c r="A5">
         <v>4</v>
       </c>
@@ -1237,7 +1237,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="6" ht="28.8" spans="1:6">
+    <row r="6" ht="30" customHeight="1" spans="1:6">
       <c r="A6">
         <v>5</v>
       </c>
@@ -1257,7 +1257,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="7" spans="1:6">
+    <row r="7" ht="30" customHeight="1" spans="1:6">
       <c r="A7">
         <v>6</v>
       </c>
@@ -1277,7 +1277,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="8" spans="1:6">
+    <row r="8" ht="30" customHeight="1" spans="1:6">
       <c r="A8">
         <v>7</v>
       </c>
@@ -1297,7 +1297,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="9" ht="72" spans="1:6">
+    <row r="9" ht="30" customHeight="1" spans="1:6">
       <c r="A9">
         <v>9</v>
       </c>
@@ -1317,7 +1317,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="10" ht="72" spans="1:6">
+    <row r="10" ht="30" customHeight="1" spans="1:6">
       <c r="A10">
         <v>10</v>
       </c>
@@ -1337,7 +1337,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="11" ht="72" spans="1:6">
+    <row r="11" ht="30" customHeight="1" spans="1:6">
       <c r="A11">
         <v>11</v>
       </c>
@@ -1357,7 +1357,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="12" ht="72" spans="1:6">
+    <row r="12" ht="30" customHeight="1" spans="1:6">
       <c r="A12">
         <v>12</v>
       </c>
@@ -1377,7 +1377,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="13" ht="43.2" spans="1:6">
+    <row r="13" ht="30" customHeight="1" spans="1:6">
       <c r="A13">
         <v>13</v>
       </c>
@@ -1397,7 +1397,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="14" ht="72" spans="1:6">
+    <row r="14" ht="30" customHeight="1" spans="1:6">
       <c r="A14">
         <v>14</v>
       </c>
@@ -1417,7 +1417,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="15" ht="72" spans="1:6">
+    <row r="15" ht="30" customHeight="1" spans="1:6">
       <c r="A15">
         <v>15</v>
       </c>
@@ -1437,7 +1437,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="16" ht="72" spans="1:6">
+    <row r="16" ht="30" customHeight="1" spans="1:6">
       <c r="A16">
         <v>16</v>
       </c>
@@ -1457,7 +1457,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="17" ht="43.2" spans="1:6">
+    <row r="17" ht="30" customHeight="1" spans="1:6">
       <c r="A17">
         <v>17</v>
       </c>
@@ -1477,7 +1477,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="18" ht="43.2" spans="1:6">
+    <row r="18" ht="30" customHeight="1" spans="1:6">
       <c r="A18">
         <v>18</v>
       </c>

</xml_diff>